<commit_message>
Databases and preprocessed files
</commit_message>
<xml_diff>
--- a/scripts/info_original_datasets.xlsx
+++ b/scripts/info_original_datasets.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProtoQSAR\COMPIS\ONTOX_2022\ONTOX_2022_T3.1\MANUSCRIPT\first_final_version\Processing_datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique\Documents\GitHub\IRB\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6969D2AC-C512-434B-826D-A0AE93651FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE4B145-43C3-43D7-B0CC-F894124D91B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D90B3C00-3DFA-4F73-8988-762800ADCE82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D90B3C00-3DFA-4F73-8988-762800ADCE82}"/>
   </bookViews>
   <sheets>
-    <sheet name="Needed info" sheetId="1" r:id="rId1"/>
+    <sheet name="Needed info_RESERVA" sheetId="1" r:id="rId1"/>
     <sheet name="all_info" sheetId="2" r:id="rId2"/>
     <sheet name="readme" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="572">
   <si>
     <t>dataset</t>
   </si>
@@ -1682,6 +1682,69 @@
   </si>
   <si>
     <t>pka_type</t>
+  </si>
+  <si>
+    <t>IRB</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp3a4_inhibitor</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp3a4_inhibitor_all.csv</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp2d6_inhibitor</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp2c9_inhibitor</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp2c19_inhibitor</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp1a2_inhibitor</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp2c9_inhibitor_all.csv</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp2c19_inhibitor_all.csv</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp2d6_inhibitor_all.csv</t>
+  </si>
+  <si>
+    <t>DeppPK_cyp1a2_inhibitor_all.csv</t>
+  </si>
+  <si>
+    <t>classCYP3A4inh</t>
+  </si>
+  <si>
+    <t>classCYP2C9inh</t>
+  </si>
+  <si>
+    <t>classCYP2C19inh</t>
+  </si>
+  <si>
+    <t>classCYP2D6inh</t>
+  </si>
+  <si>
+    <t>classCYP1A2inh</t>
+  </si>
+  <si>
+    <t>IRB_CYP3A4inh_DeepPK</t>
+  </si>
+  <si>
+    <t>IRB_CYP2C9inh_DeepPK</t>
+  </si>
+  <si>
+    <t>IRB_CYP2D6inh_DeepPK</t>
+  </si>
+  <si>
+    <t>IRB_CYP1A2inh_DeepPK</t>
+  </si>
+  <si>
+    <t>IRB_CYP2C19inh_DeepPK</t>
   </si>
 </sst>
 </file>
@@ -2010,9 +2073,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2050,7 +2113,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2156,7 +2219,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2298,7 +2361,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2308,9 +2371,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7C953B-D8D2-4E2A-8385-F60286660B13}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22:E25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="31.42578125" defaultRowHeight="18.75"/>
@@ -3368,9 +3431,7 @@
       <c r="D21" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="E21" s="14"/>
       <c r="F21" s="27" t="s">
         <v>26</v>
       </c>
@@ -3427,9 +3488,7 @@
         <v>26</v>
       </c>
       <c r="D22" s="14"/>
-      <c r="E22" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="E22" s="14"/>
       <c r="F22" s="14" t="s">
         <v>26</v>
       </c>
@@ -3487,9 +3546,7 @@
         <v>26</v>
       </c>
       <c r="D23" s="14"/>
-      <c r="E23" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="E23" s="14"/>
       <c r="F23" s="14" t="s">
         <v>26</v>
       </c>
@@ -3551,9 +3608,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="14"/>
-      <c r="E24" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="E24" s="14"/>
       <c r="F24" s="14" t="s">
         <v>26</v>
       </c>
@@ -3613,9 +3668,7 @@
       <c r="D25" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="E25" s="14"/>
       <c r="F25" s="27" t="s">
         <v>26</v>
       </c>
@@ -5186,17 +5239,105 @@
         <v>547</v>
       </c>
     </row>
+    <row r="61" spans="1:25">
+      <c r="A61" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="T61" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="U61" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="W61" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25">
+      <c r="A62" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="T62" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="U62" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="W62" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
     <row r="63" spans="1:25">
+      <c r="A63" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>556</v>
+      </c>
       <c r="C63"/>
       <c r="D63"/>
-      <c r="E63"/>
+      <c r="E63" t="s">
+        <v>26</v>
+      </c>
       <c r="F63"/>
       <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
-      <c r="J63"/>
-      <c r="K63"/>
-      <c r="L63"/>
+      <c r="H63" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="M63"/>
       <c r="N63"/>
       <c r="O63"/>
@@ -5204,19 +5345,45 @@
       <c r="Q63"/>
       <c r="R63"/>
       <c r="S63"/>
-      <c r="T63"/>
+      <c r="T63" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="U63" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="W63" s="2" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="64" spans="1:25">
+      <c r="A64" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>554</v>
+      </c>
       <c r="C64"/>
       <c r="D64"/>
-      <c r="E64"/>
+      <c r="E64" t="s">
+        <v>26</v>
+      </c>
       <c r="F64"/>
       <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
-      <c r="J64"/>
-      <c r="K64"/>
-      <c r="L64"/>
+      <c r="H64" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="M64"/>
       <c r="N64"/>
       <c r="O64"/>
@@ -5224,9 +5391,52 @@
       <c r="Q64"/>
       <c r="R64"/>
       <c r="S64"/>
-      <c r="T64"/>
-    </row>
-    <row r="66" spans="15:15">
+      <c r="T64" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="U64" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="W64" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23">
+      <c r="A65" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="T65" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="U65" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="W65" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23">
       <c r="O66"/>
     </row>
   </sheetData>
@@ -5240,7 +5450,7 @@
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.85546875" defaultRowHeight="38.450000000000003" customHeight="1"/>
@@ -7775,8 +7985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7026E883-5A86-496E-8610-33338E970ECC}">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>